<commit_message>
correctly deletes only subplate data when selected
</commit_message>
<xml_diff>
--- a/data-raw/2024-use-case/2024 JPE Events 3+4 Files + Plating Scheme v5 (1)/080124_JPE24_EL_E3-4_P1_SH_reruns.xlsx
+++ b/data-raw/2024-use-case/2024 JPE Events 3+4 Files + Plating Scheme v5 (1)/080124_JPE24_EL_E3-4_P1_SH_reruns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canfi\OneDrive\Desktop\GVL-DWR_Stuff\JPE\2024\Results\SHERLOCK\E3+4\Ots28\GrunID Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanuel\projects\jpe\grunID\data-raw\2024-use-case\2024 JPE Events 3+4 Files + Plating Scheme v5 (1)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BF4D87-AF88-4906-AAD3-42CFA384D1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1070620-4661-4CAA-A799-4448366C4658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4380" yWindow="4716" windowWidth="36720" windowHeight="20532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sherlock_output" sheetId="1" r:id="rId1"/>
@@ -893,9 +893,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -933,7 +933,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1039,7 +1039,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1181,7 +1181,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1191,17 +1191,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AS205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>45299</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>0.5290393518518518</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1273,13 +1273,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1287,12 +1287,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1300,12 +1300,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1321,53 +1321,53 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B29" s="4"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="6">
         <v>1</v>
@@ -1442,7 +1442,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>36</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>41</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>42</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>46</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>47</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B37" s="6" t="s">
         <v>51</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
         <v>52</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>56</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>59</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>63</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>66</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>70</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>73</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
         <v>77</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
         <v>79</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="2:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
         <v>81</v>
       </c>
@@ -2038,13 +2038,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
         <v>484530</v>
       </c>
       <c r="B49" s="4"/>
     </row>
-    <row r="51" spans="1:45" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:45" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
         <v>9</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B52" s="12">
         <v>0</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>2388</v>
       </c>
     </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B53" s="12">
         <v>2.0833333333333333E-3</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B54" s="12">
         <v>4.1666666666666666E-3</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>2836</v>
       </c>
     </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B55" s="12">
         <v>6.2499999999999995E-3</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>2981</v>
       </c>
     </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B56" s="12">
         <v>8.3333333333333332E-3</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>3182</v>
       </c>
     </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B57" s="12">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>3299</v>
       </c>
     </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B58" s="12">
         <v>1.2499999999999999E-2</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>3517</v>
       </c>
     </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B59" s="12">
         <v>1.4583333333333332E-2</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>3709</v>
       </c>
     </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B60" s="12">
         <v>1.6666666666666666E-2</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>3738</v>
       </c>
     </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B61" s="12">
         <v>1.8749999999999999E-2</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>3872</v>
       </c>
     </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B62" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>4029</v>
       </c>
     </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B63" s="12">
         <v>2.2916666666666669E-2</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>4088</v>
       </c>
     </row>
-    <row r="64" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B64" s="12">
         <v>2.4999999999999998E-2</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>4221</v>
       </c>
     </row>
-    <row r="65" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B65" s="12">
         <v>2.7083333333333334E-2</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>4269</v>
       </c>
     </row>
-    <row r="66" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B66" s="12">
         <v>2.9166666666666664E-2</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>4319</v>
       </c>
     </row>
-    <row r="67" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B67" s="12">
         <v>3.125E-2</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>4499</v>
       </c>
     </row>
-    <row r="68" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B68" s="12">
         <v>3.3333333333333333E-2</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>4592</v>
       </c>
     </row>
-    <row r="69" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B69" s="12">
         <v>3.5416666666666666E-2</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>4488</v>
       </c>
     </row>
-    <row r="70" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B70" s="12">
         <v>3.7499999999999999E-2</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>4675</v>
       </c>
     </row>
-    <row r="71" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B71" s="12">
         <v>3.9583333333333331E-2</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>4781</v>
       </c>
     </row>
-    <row r="72" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B72" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>4893</v>
       </c>
     </row>
-    <row r="73" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B73" s="12">
         <v>4.3750000000000004E-2</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>4940</v>
       </c>
     </row>
-    <row r="74" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B74" s="12">
         <v>4.5833333333333337E-2</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>4955</v>
       </c>
     </row>
-    <row r="75" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B75" s="12">
         <v>4.7916666666666663E-2</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>5071</v>
       </c>
     </row>
-    <row r="76" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B76" s="12">
         <v>4.9999999999999996E-2</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>5258</v>
       </c>
     </row>
-    <row r="77" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B77" s="12">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>5374</v>
       </c>
     </row>
-    <row r="78" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B78" s="12">
         <v>5.4166666666666669E-2</v>
       </c>
@@ -5796,7 +5796,7 @@
         <v>5211</v>
       </c>
     </row>
-    <row r="79" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B79" s="12">
         <v>5.6250000000000001E-2</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>5385</v>
       </c>
     </row>
-    <row r="80" spans="2:45" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B80" s="12">
         <v>5.8333333333333327E-2</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>5420</v>
       </c>
     </row>
-    <row r="81" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B81" s="12">
         <v>6.0416666666666667E-2</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>5622</v>
       </c>
     </row>
-    <row r="82" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B82" s="12">
         <v>6.25E-2</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>5672</v>
       </c>
     </row>
-    <row r="83" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B83" s="12">
         <v>6.458333333333334E-2</v>
       </c>
@@ -6466,7 +6466,7 @@
         <v>5689</v>
       </c>
     </row>
-    <row r="84" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B84" s="12">
         <v>6.6666666666666666E-2</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v>5701</v>
       </c>
     </row>
-    <row r="85" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B85" s="12">
         <v>6.8749999999999992E-2</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>5869</v>
       </c>
     </row>
-    <row r="86" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B86" s="12">
         <v>7.0833333333333331E-2</v>
       </c>
@@ -6868,7 +6868,7 @@
         <v>5907</v>
       </c>
     </row>
-    <row r="87" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B87" s="12">
         <v>7.2916666666666671E-2</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>5882</v>
       </c>
     </row>
-    <row r="88" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B88" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v>5916</v>
       </c>
     </row>
-    <row r="89" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B89" s="12">
         <v>7.7083333333333337E-2</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>6020</v>
       </c>
     </row>
-    <row r="90" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B90" s="12">
         <v>7.9166666666666663E-2</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>6123</v>
       </c>
     </row>
-    <row r="91" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B91" s="12">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -7538,7 +7538,7 @@
         <v>6253</v>
       </c>
     </row>
-    <row r="92" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B92" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -7549,7 +7549,7 @@
         <v>31278</v>
       </c>
       <c r="E92" s="13">
-        <v>4332</v>
+        <v>44332</v>
       </c>
       <c r="F92" s="13">
         <v>5137</v>
@@ -7672,13 +7672,13 @@
         <v>6273</v>
       </c>
     </row>
-    <row r="94" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>125</v>
       </c>
       <c r="B94" s="4"/>
     </row>
-    <row r="96" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B96" s="6" t="s">
         <v>9</v>
       </c>
@@ -7809,7 +7809,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="97" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B97" s="12">
         <v>0</v>
       </c>
@@ -7940,7 +7940,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="98" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B98" s="12">
         <v>2.0833333333333333E-3</v>
       </c>
@@ -8071,7 +8071,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="99" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B99" s="12">
         <v>4.1666666666666666E-3</v>
       </c>
@@ -8202,7 +8202,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="100" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B100" s="12">
         <v>6.2499999999999995E-3</v>
       </c>
@@ -8333,7 +8333,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="101" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B101" s="12">
         <v>8.3333333333333332E-3</v>
       </c>
@@ -8464,7 +8464,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="102" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B102" s="12">
         <v>1.0416666666666666E-2</v>
       </c>
@@ -8595,7 +8595,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="103" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B103" s="12">
         <v>1.2499999999999999E-2</v>
       </c>
@@ -8726,7 +8726,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="104" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B104" s="12">
         <v>1.4583333333333332E-2</v>
       </c>
@@ -8857,7 +8857,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="105" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B105" s="12">
         <v>1.6666666666666666E-2</v>
       </c>
@@ -8988,7 +8988,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="106" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B106" s="12">
         <v>1.8749999999999999E-2</v>
       </c>
@@ -9119,7 +9119,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="107" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B107" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -9250,7 +9250,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="108" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B108" s="12">
         <v>2.2916666666666669E-2</v>
       </c>
@@ -9381,7 +9381,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="109" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B109" s="12">
         <v>2.4999999999999998E-2</v>
       </c>
@@ -9512,7 +9512,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="110" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B110" s="12">
         <v>2.7083333333333334E-2</v>
       </c>
@@ -9643,7 +9643,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="111" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B111" s="12">
         <v>2.9166666666666664E-2</v>
       </c>
@@ -9774,7 +9774,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="112" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B112" s="12">
         <v>3.125E-2</v>
       </c>
@@ -9905,7 +9905,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="113" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B113" s="12">
         <v>3.3333333333333333E-2</v>
       </c>
@@ -10036,7 +10036,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="114" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B114" s="12">
         <v>3.5416666666666666E-2</v>
       </c>
@@ -10167,7 +10167,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="115" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B115" s="12">
         <v>3.7499999999999999E-2</v>
       </c>
@@ -10298,7 +10298,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="116" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B116" s="12">
         <v>3.9583333333333331E-2</v>
       </c>
@@ -10429,7 +10429,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="117" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B117" s="12">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -10560,7 +10560,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="118" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B118" s="12">
         <v>4.3750000000000004E-2</v>
       </c>
@@ -10691,7 +10691,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="119" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B119" s="12">
         <v>4.5833333333333337E-2</v>
       </c>
@@ -10822,7 +10822,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="120" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B120" s="12">
         <v>4.7916666666666663E-2</v>
       </c>
@@ -10953,7 +10953,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="121" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B121" s="12">
         <v>4.9999999999999996E-2</v>
       </c>
@@ -11084,7 +11084,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="122" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B122" s="12">
         <v>5.2083333333333336E-2</v>
       </c>
@@ -11215,7 +11215,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="123" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B123" s="12">
         <v>5.4166666666666669E-2</v>
       </c>
@@ -11346,7 +11346,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="124" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B124" s="12">
         <v>5.6250000000000001E-2</v>
       </c>
@@ -11477,7 +11477,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="125" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B125" s="12">
         <v>5.8333333333333327E-2</v>
       </c>
@@ -11608,7 +11608,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="126" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B126" s="12">
         <v>6.0416666666666667E-2</v>
       </c>
@@ -11739,7 +11739,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="127" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B127" s="12">
         <v>6.25E-2</v>
       </c>
@@ -11870,7 +11870,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="128" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B128" s="12">
         <v>6.458333333333334E-2</v>
       </c>
@@ -12001,7 +12001,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="129" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B129" s="12">
         <v>6.6666666666666666E-2</v>
       </c>
@@ -12132,7 +12132,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="130" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B130" s="12">
         <v>6.8749999999999992E-2</v>
       </c>
@@ -12263,7 +12263,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="131" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B131" s="12">
         <v>7.0833333333333331E-2</v>
       </c>
@@ -12394,7 +12394,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="132" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B132" s="12">
         <v>7.2916666666666671E-2</v>
       </c>
@@ -12525,7 +12525,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="133" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B133" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -12656,7 +12656,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="134" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B134" s="12">
         <v>7.7083333333333337E-2</v>
       </c>
@@ -12787,7 +12787,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="135" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B135" s="12">
         <v>7.9166666666666663E-2</v>
       </c>
@@ -12918,7 +12918,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="136" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B136" s="12">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -13049,7 +13049,7 @@
         <v>1276</v>
       </c>
     </row>
-    <row r="137" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B137" s="12">
         <v>8.3333333333333329E-2</v>
       </c>
@@ -13180,13 +13180,13 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="139" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B139" s="4"/>
     </row>
-    <row r="141" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B141" s="5"/>
       <c r="C141" s="6">
         <v>1</v>
@@ -13261,7 +13261,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="142" spans="1:44" ht="18" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:44" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B142" s="31" t="s">
         <v>36</v>
       </c>
@@ -13301,7 +13301,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="143" spans="1:44" ht="27" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:44" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B143" s="32"/>
       <c r="C143" s="15">
         <v>0.999</v>
@@ -13339,7 +13339,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="144" spans="1:44" ht="27" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:44" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B144" s="32"/>
       <c r="C144" s="16">
         <v>4.3750000000000004E-2</v>
@@ -13377,7 +13377,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="145" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B145" s="33"/>
       <c r="C145" s="17">
         <v>2.7210648148148147E-2</v>
@@ -13415,7 +13415,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="146" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B146" s="31" t="s">
         <v>41</v>
       </c>
@@ -13447,7 +13447,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="147" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B147" s="32"/>
       <c r="C147" s="15"/>
       <c r="D147" s="15"/>
@@ -13477,7 +13477,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="148" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B148" s="32"/>
       <c r="C148" s="15"/>
       <c r="D148" s="15"/>
@@ -13507,7 +13507,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="149" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B149" s="33"/>
       <c r="C149" s="18"/>
       <c r="D149" s="18"/>
@@ -13537,7 +13537,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="150" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B150" s="31" t="s">
         <v>42</v>
       </c>
@@ -13577,7 +13577,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="151" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B151" s="32"/>
       <c r="C151" s="15">
         <v>0.99099999999999999</v>
@@ -13615,7 +13615,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="152" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B152" s="32"/>
       <c r="C152" s="16">
         <v>1.6666666666666666E-2</v>
@@ -13653,7 +13653,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="153" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B153" s="33"/>
       <c r="C153" s="17">
         <v>1.224537037037037E-2</v>
@@ -13691,7 +13691,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="154" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B154" s="31" t="s">
         <v>46</v>
       </c>
@@ -13723,7 +13723,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="155" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B155" s="32"/>
       <c r="C155" s="15"/>
       <c r="D155" s="15"/>
@@ -13753,7 +13753,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="156" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B156" s="32"/>
       <c r="C156" s="15"/>
       <c r="D156" s="15"/>
@@ -13783,7 +13783,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="157" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B157" s="33"/>
       <c r="C157" s="18"/>
       <c r="D157" s="18"/>
@@ -13813,7 +13813,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="158" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B158" s="31" t="s">
         <v>47</v>
       </c>
@@ -13853,7 +13853,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="159" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B159" s="32"/>
       <c r="C159" s="15">
         <v>0.82599999999999996</v>
@@ -13891,7 +13891,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="160" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B160" s="32"/>
       <c r="C160" s="16">
         <v>4.1666666666666666E-3</v>
@@ -13929,7 +13929,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="161" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B161" s="33"/>
       <c r="C161" s="17">
         <v>1.7939814814814815E-3</v>
@@ -13967,7 +13967,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="162" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B162" s="31" t="s">
         <v>51</v>
       </c>
@@ -13999,7 +13999,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="163" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B163" s="32"/>
       <c r="C163" s="15"/>
       <c r="D163" s="15"/>
@@ -14029,7 +14029,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="164" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B164" s="32"/>
       <c r="C164" s="15"/>
       <c r="D164" s="15"/>
@@ -14059,7 +14059,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="165" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B165" s="33"/>
       <c r="C165" s="18"/>
       <c r="D165" s="18"/>
@@ -14089,7 +14089,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="166" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B166" s="31" t="s">
         <v>52</v>
       </c>
@@ -14129,7 +14129,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="167" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B167" s="32"/>
       <c r="C167" s="15">
         <v>0.96799999999999997</v>
@@ -14167,7 +14167,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="168" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B168" s="32"/>
       <c r="C168" s="16">
         <v>1.4583333333333332E-2</v>
@@ -14205,7 +14205,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="169" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B169" s="33"/>
       <c r="C169" s="17">
         <v>1.1111111111111112E-2</v>
@@ -14243,7 +14243,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="170" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B170" s="31" t="s">
         <v>56</v>
       </c>
@@ -14279,7 +14279,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="171" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B171" s="32"/>
       <c r="C171" s="15"/>
       <c r="D171" s="15"/>
@@ -14313,7 +14313,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="172" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B172" s="32"/>
       <c r="C172" s="15"/>
       <c r="D172" s="15"/>
@@ -14347,7 +14347,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="173" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B173" s="33"/>
       <c r="C173" s="18"/>
       <c r="D173" s="18"/>
@@ -14381,7 +14381,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="174" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B174" s="31" t="s">
         <v>59</v>
       </c>
@@ -14421,7 +14421,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="175" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B175" s="32"/>
       <c r="C175" s="15">
         <v>0.998</v>
@@ -14459,7 +14459,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="176" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B176" s="32"/>
       <c r="C176" s="16">
         <v>4.1666666666666666E-3</v>
@@ -14497,7 +14497,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="177" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B177" s="33"/>
       <c r="C177" s="17">
         <v>1.1574074074074073E-4</v>
@@ -14535,7 +14535,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="178" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B178" s="31" t="s">
         <v>63</v>
       </c>
@@ -14571,7 +14571,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="179" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B179" s="32"/>
       <c r="C179" s="15"/>
       <c r="D179" s="15"/>
@@ -14605,7 +14605,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="180" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B180" s="32"/>
       <c r="C180" s="15"/>
       <c r="D180" s="15"/>
@@ -14639,7 +14639,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="181" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B181" s="33"/>
       <c r="C181" s="18"/>
       <c r="D181" s="18"/>
@@ -14673,7 +14673,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="182" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B182" s="31" t="s">
         <v>66</v>
       </c>
@@ -14713,7 +14713,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="183" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B183" s="32"/>
       <c r="C183" s="15">
         <v>0.85799999999999998</v>
@@ -14751,7 +14751,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="184" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B184" s="32"/>
       <c r="C184" s="16">
         <v>4.1666666666666666E-3</v>
@@ -14789,7 +14789,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="185" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B185" s="33"/>
       <c r="C185" s="18" t="s">
         <v>131</v>
@@ -14827,7 +14827,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="186" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B186" s="31" t="s">
         <v>70</v>
       </c>
@@ -14863,7 +14863,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="187" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B187" s="32"/>
       <c r="C187" s="15"/>
       <c r="D187" s="15"/>
@@ -14897,7 +14897,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="188" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B188" s="32"/>
       <c r="C188" s="15"/>
       <c r="D188" s="15"/>
@@ -14931,7 +14931,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="189" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B189" s="33"/>
       <c r="C189" s="18"/>
       <c r="D189" s="18"/>
@@ -14965,7 +14965,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="190" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B190" s="31" t="s">
         <v>73</v>
       </c>
@@ -15005,7 +15005,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="191" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B191" s="32"/>
       <c r="C191" s="15">
         <v>0.99399999999999999</v>
@@ -15043,7 +15043,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="192" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B192" s="32"/>
       <c r="C192" s="16">
         <v>4.1666666666666666E-3</v>
@@ -15081,7 +15081,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="193" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B193" s="33"/>
       <c r="C193" s="18" t="s">
         <v>131</v>
@@ -15119,7 +15119,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="194" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B194" s="31" t="s">
         <v>77</v>
       </c>
@@ -15155,7 +15155,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="195" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B195" s="32"/>
       <c r="C195" s="15"/>
       <c r="D195" s="15"/>
@@ -15189,7 +15189,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="196" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B196" s="32"/>
       <c r="C196" s="15"/>
       <c r="D196" s="15"/>
@@ -15223,7 +15223,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="197" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B197" s="33"/>
       <c r="C197" s="18"/>
       <c r="D197" s="18"/>
@@ -15257,7 +15257,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="198" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B198" s="31" t="s">
         <v>79</v>
       </c>
@@ -15297,7 +15297,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="199" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B199" s="32"/>
       <c r="C199" s="15">
         <v>0.85299999999999998</v>
@@ -15335,7 +15335,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="200" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B200" s="32"/>
       <c r="C200" s="16">
         <v>4.1666666666666666E-3</v>
@@ -15373,7 +15373,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="201" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B201" s="33"/>
       <c r="C201" s="18" t="s">
         <v>131</v>
@@ -15411,7 +15411,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="202" spans="2:27" ht="18" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:27" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B202" s="31" t="s">
         <v>81</v>
       </c>
@@ -15447,7 +15447,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="203" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B203" s="32"/>
       <c r="C203" s="15"/>
       <c r="D203" s="15"/>
@@ -15481,7 +15481,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="204" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B204" s="32"/>
       <c r="C204" s="15"/>
       <c r="D204" s="15"/>
@@ -15515,7 +15515,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="205" spans="2:27" ht="27" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:27" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B205" s="33"/>
       <c r="C205" s="18"/>
       <c r="D205" s="18"/>
@@ -15551,11 +15551,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B142:B145"/>
-    <mergeCell ref="B146:B149"/>
-    <mergeCell ref="B150:B153"/>
-    <mergeCell ref="B154:B157"/>
-    <mergeCell ref="B158:B161"/>
     <mergeCell ref="B162:B165"/>
     <mergeCell ref="B190:B193"/>
     <mergeCell ref="B194:B197"/>
@@ -15567,6 +15562,11 @@
     <mergeCell ref="B178:B181"/>
     <mergeCell ref="B182:B185"/>
     <mergeCell ref="B186:B189"/>
+    <mergeCell ref="B142:B145"/>
+    <mergeCell ref="B146:B149"/>
+    <mergeCell ref="B150:B153"/>
+    <mergeCell ref="B154:B157"/>
+    <mergeCell ref="B158:B161"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15579,16 +15579,16 @@
   <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y29" sqref="Y29"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="25" width="15.85546875" customWidth="1"/>
+    <col min="2" max="25" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="19">
         <v>1</v>
       </c>
@@ -15662,7 +15662,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>36</v>
       </c>
@@ -15701,7 +15701,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>41</v>
       </c>
@@ -15730,7 +15730,7 @@
       <c r="X3" s="23"/>
       <c r="Y3" s="24"/>
     </row>
-    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>42</v>
       </c>
@@ -15769,7 +15769,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>46</v>
       </c>
@@ -15798,7 +15798,7 @@
       <c r="X5" s="23"/>
       <c r="Y5" s="24"/>
     </row>
-    <row r="6" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>47</v>
       </c>
@@ -15837,7 +15837,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>51</v>
       </c>
@@ -15866,7 +15866,7 @@
       <c r="X7" s="23"/>
       <c r="Y7" s="24"/>
     </row>
-    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>52</v>
       </c>
@@ -15905,7 +15905,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>56</v>
       </c>
@@ -15938,7 +15938,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>59</v>
       </c>
@@ -15977,7 +15977,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>63</v>
       </c>
@@ -16010,7 +16010,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>66</v>
       </c>
@@ -16049,7 +16049,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>70</v>
       </c>
@@ -16082,7 +16082,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>73</v>
       </c>
@@ -16121,7 +16121,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>77</v>
       </c>
@@ -16154,7 +16154,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>79</v>
       </c>
@@ -16193,7 +16193,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
         <v>81</v>
       </c>
@@ -16226,7 +16226,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="14.4" x14ac:dyDescent="0.3">
       <c r="N18" s="30"/>
     </row>
   </sheetData>
@@ -16235,26 +16235,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a707c639-4ab7-466f-ab80-9083af4ef22b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="02ee1384-56f9-49a7-aa58-df62156adfc7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009AE391E1779C514D98B0AAF78991A34A" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20865b83f50b8ce2b19f31cddc80d719">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a707c639-4ab7-466f-ab80-9083af4ef22b" xmlns:ns3="02ee1384-56f9-49a7-aa58-df62156adfc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0acb1623640e290c6f9e9b40375a9f1" ns2:_="" ns3:_="">
     <xsd:import namespace="a707c639-4ab7-466f-ab80-9083af4ef22b"/>
@@ -16483,10 +16463,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a707c639-4ab7-466f-ab80-9083af4ef22b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="02ee1384-56f9-49a7-aa58-df62156adfc7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{093EDFFE-31B9-44D2-8BC9-D47699D569CD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C154929-882F-4007-91E8-592C3E044DED}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a707c639-4ab7-466f-ab80-9083af4ef22b"/>
+    <ds:schemaRef ds:uri="02ee1384-56f9-49a7-aa58-df62156adfc7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16503,20 +16514,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C154929-882F-4007-91E8-592C3E044DED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{093EDFFE-31B9-44D2-8BC9-D47699D569CD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a707c639-4ab7-466f-ab80-9083af4ef22b"/>
-    <ds:schemaRef ds:uri="02ee1384-56f9-49a7-aa58-df62156adfc7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>